<commit_message>
Work in progress, toglierò un po' di files a breve
</commit_message>
<xml_diff>
--- a/Dataset 2.xlsx
+++ b/Dataset 2.xlsx
@@ -350,7 +350,7 @@
   <dimension ref="A1:A997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -362,7 +362,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>7.5181801655310274E-3</v>
+        <v>7.5181801655310283E-3</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -377,12 +377,12 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>-2.8074030247972784E-3</v>
+        <v>-2.8074030247972779E-3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>1.5053863582353859E-3</v>
+        <v>1.5053863582353856E-3</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -392,7 +392,7 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-1.0647373591979729E-3</v>
+        <v>-1.0647373591979726E-3</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -402,7 +402,7 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>4.451898996075108E-3</v>
+        <v>4.4518989960751088E-3</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -427,12 +427,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>-6.4945916019624227E-3</v>
+        <v>-6.4945916019624236E-3</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>-5.1301941774983166E-4</v>
+        <v>-5.1301941774983156E-4</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -442,7 +442,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>1.4242356377185508E-3</v>
+        <v>1.424235637718551E-3</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -487,27 +487,27 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>6.1839278951495921E-3</v>
+        <v>6.183927895149593E-3</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>1.0674536887663488E-3</v>
+        <v>1.0674536887663485E-3</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>-7.8708524981896703E-4</v>
+        <v>-7.8708524981896714E-4</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>7.2948651762984136E-3</v>
+        <v>7.2948651762984144E-3</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>1.8644516718518192E-3</v>
+        <v>1.864451671851819E-3</v>
       </c>
     </row>
     <row r="32" spans="1:1">
@@ -517,17 +517,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>-8.13299066779848E-5</v>
+        <v>-8.1329906677984787E-5</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>6.7483792223020493E-4</v>
+        <v>6.7483792223020482E-4</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>5.196417174860476E-3</v>
+        <v>5.1964171748604751E-3</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -542,12 +542,12 @@
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>-5.6238306241261984E-4</v>
+        <v>-5.6238306241261974E-4</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>2.5464024624049673E-3</v>
+        <v>2.5464024624049669E-3</v>
       </c>
     </row>
     <row r="40" spans="1:1">
@@ -557,17 +557,17 @@
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>-9.6501524662406031E-4</v>
+        <v>-9.6501524662406042E-4</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>-1.3542058238749353E-3</v>
+        <v>-1.3542058238749351E-3</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>-4.9767650840993813E-4</v>
+        <v>-4.9767650840993824E-4</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -577,7 +577,7 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>3.956926085374805E-4</v>
+        <v>3.9569260853748056E-4</v>
       </c>
     </row>
     <row r="46" spans="1:1">
@@ -587,7 +587,7 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>1.7419741249740793E-3</v>
+        <v>1.7419741249740796E-3</v>
       </c>
     </row>
     <row r="48" spans="1:1">
@@ -622,7 +622,7 @@
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>-2.1095163606313155E-4</v>
+        <v>-2.1095163606313157E-4</v>
       </c>
     </row>
     <row r="55" spans="1:1">
@@ -657,7 +657,7 @@
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>-2.0888891023388813E-3</v>
+        <v>-2.0888891023388818E-3</v>
       </c>
     </row>
     <row r="62" spans="1:1">
@@ -667,7 +667,7 @@
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>2.2915413580277687E-4</v>
+        <v>2.2915413580277684E-4</v>
       </c>
     </row>
     <row r="64" spans="1:1">
@@ -682,7 +682,7 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>5.7536951033113452E-3</v>
+        <v>5.7536951033113444E-3</v>
       </c>
     </row>
     <row r="67" spans="1:1">
@@ -717,7 +717,7 @@
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>3.5267602631470244E-3</v>
+        <v>3.5267602631470249E-3</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -732,12 +732,12 @@
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>1.4411474025610078E-3</v>
+        <v>1.4411474025610076E-3</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>1.7226464262413755E-3</v>
+        <v>1.7226464262413753E-3</v>
       </c>
     </row>
     <row r="78" spans="1:1">
@@ -762,7 +762,7 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
-        <v>-2.0326592812422327E-3</v>
+        <v>-2.0326592812422322E-3</v>
       </c>
     </row>
     <row r="83" spans="1:1">
@@ -777,7 +777,7 @@
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
-        <v>1.0723476868888583E-3</v>
+        <v>1.0723476868888585E-3</v>
       </c>
     </row>
     <row r="86" spans="1:1">
@@ -807,7 +807,7 @@
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
-        <v>-1.2742326433829215E-3</v>
+        <v>-1.2742326433829217E-3</v>
       </c>
     </row>
     <row r="92" spans="1:1">
@@ -822,7 +822,7 @@
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
-        <v>1.6608436514402966E-3</v>
+        <v>1.6608436514402968E-3</v>
       </c>
     </row>
     <row r="95" spans="1:1">
@@ -867,7 +867,7 @@
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
-        <v>1.5346566589212428E-3</v>
+        <v>1.534656658921243E-3</v>
       </c>
     </row>
     <row r="104" spans="1:1">
@@ -877,7 +877,7 @@
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <v>1.2505863752767118E-3</v>
+        <v>1.250586375276712E-3</v>
       </c>
     </row>
     <row r="106" spans="1:1">
@@ -892,12 +892,12 @@
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
-        <v>9.4407985457522201E-4</v>
+        <v>9.4407985457522191E-4</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
-        <v>1.6296443610471806E-3</v>
+        <v>1.6296443610471804E-3</v>
       </c>
     </row>
     <row r="110" spans="1:1">
@@ -907,12 +907,12 @@
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
-        <v>3.1039218675159492E-3</v>
+        <v>3.1039218675159488E-3</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
-        <v>1.293678726408094E-3</v>
+        <v>1.2936787264080942E-3</v>
       </c>
     </row>
     <row r="113" spans="1:1">
@@ -932,12 +932,12 @@
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
-        <v>-8.9024108187553928E-4</v>
+        <v>-8.9024108187553918E-4</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
-        <v>9.6761590878809535E-4</v>
+        <v>9.6761590878809546E-4</v>
       </c>
     </row>
     <row r="118" spans="1:1">
@@ -957,17 +957,17 @@
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
-        <v>-2.6721209291354253E-3</v>
+        <v>-2.6721209291354249E-3</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
-        <v>1.3524434200012513E-3</v>
+        <v>1.3524434200012515E-3</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
-        <v>6.5541101160685221E-3</v>
+        <v>6.554110116068523E-3</v>
       </c>
     </row>
     <row r="124" spans="1:1">
@@ -982,7 +982,7 @@
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
-        <v>-3.5357961290138348E-4</v>
+        <v>-3.5357961290138353E-4</v>
       </c>
     </row>
     <row r="127" spans="1:1">
@@ -1007,7 +1007,7 @@
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
-        <v>-1.0377177203096622E-3</v>
+        <v>-1.0377177203096625E-3</v>
       </c>
     </row>
     <row r="132" spans="1:1">
@@ -1017,7 +1017,7 @@
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
-        <v>-2.2818720479210439E-5</v>
+        <v>-2.2818720479210435E-5</v>
       </c>
     </row>
     <row r="134" spans="1:1">
@@ -1027,7 +1027,7 @@
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
-        <v>5.4494398966853878E-3</v>
+        <v>5.4494398966853869E-3</v>
       </c>
     </row>
     <row r="136" spans="1:1">
@@ -1047,7 +1047,7 @@
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
-        <v>-4.115944350004808E-3</v>
+        <v>-4.1159443500048088E-3</v>
       </c>
     </row>
     <row r="140" spans="1:1">
@@ -1062,17 +1062,17 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
-        <v>-3.3878397902287129E-3</v>
+        <v>-3.3878397902287125E-3</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
-        <v>-8.0583488477196875E-4</v>
+        <v>-8.0583488477196864E-4</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
-        <v>2.0580665174295232E-3</v>
+        <v>2.0580665174295236E-3</v>
       </c>
     </row>
     <row r="145" spans="1:1">
@@ -1082,12 +1082,12 @@
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
-        <v>-1.2043095598637283E-3</v>
+        <v>-1.2043095598637281E-3</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
-        <v>7.4214550576368293E-4</v>
+        <v>7.4214550576368282E-4</v>
       </c>
     </row>
     <row r="148" spans="1:1">
@@ -1097,12 +1097,12 @@
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
-        <v>-4.2511680136645231E-3</v>
+        <v>-4.2511680136645223E-3</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
-        <v>7.405469336260277E-3</v>
+        <v>7.4054693362602779E-3</v>
       </c>
     </row>
     <row r="151" spans="1:1">
@@ -1112,17 +1112,17 @@
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
-        <v>4.1202128691745022E-3</v>
+        <v>4.1202128691745013E-3</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
-        <v>6.7760405908426184E-3</v>
+        <v>6.7760405908426176E-3</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
-        <v>1.8251803378990564E-3</v>
+        <v>1.8251803378990562E-3</v>
       </c>
     </row>
     <row r="155" spans="1:1">
@@ -1157,7 +1157,7 @@
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
-        <v>-1.5675747406123457E-3</v>
+        <v>-1.5675747406123455E-3</v>
       </c>
     </row>
     <row r="162" spans="1:1">
@@ -1187,7 +1187,7 @@
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
-        <v>1.1576043244174918E-2</v>
+        <v>1.1576043244174919E-2</v>
       </c>
     </row>
     <row r="168" spans="1:1">
@@ -1202,7 +1202,7 @@
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
-        <v>7.0124491549206905E-4</v>
+        <v>7.0124491549206894E-4</v>
       </c>
     </row>
     <row r="171" spans="1:1">
@@ -1227,17 +1227,17 @@
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
-        <v>-5.2001307480917967E-3</v>
+        <v>-5.2001307480917976E-3</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
-        <v>-3.81193623106501E-2</v>
+        <v>-3.8119362310650107E-2</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
-        <v>1.4851662944691141E-2</v>
+        <v>1.4851662944691143E-2</v>
       </c>
     </row>
     <row r="178" spans="1:1">
@@ -1262,12 +1262,12 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
-        <v>3.5872864027537878E-4</v>
+        <v>3.5872864027537872E-4</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
-        <v>-6.0202225758322521E-3</v>
+        <v>-6.020222575832253E-3</v>
       </c>
     </row>
     <row r="184" spans="1:1">
@@ -1277,7 +1277,7 @@
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
-        <v>9.2867866070274919E-4</v>
+        <v>9.2867866070274929E-4</v>
       </c>
     </row>
     <row r="186" spans="1:1">
@@ -1287,7 +1287,7 @@
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
-        <v>1.1582742908615374E-2</v>
+        <v>1.1582742908615372E-2</v>
       </c>
     </row>
     <row r="188" spans="1:1">
@@ -1307,7 +1307,7 @@
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
-        <v>5.4140692768552042E-3</v>
+        <v>5.4140692768552051E-3</v>
       </c>
     </row>
     <row r="192" spans="1:1">
@@ -1317,7 +1317,7 @@
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
-        <v>2.6425718778806473E-3</v>
+        <v>2.6425718778806478E-3</v>
       </c>
     </row>
     <row r="194" spans="1:1">
@@ -1342,7 +1342,7 @@
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
-        <v>-6.517217213717728E-3</v>
+        <v>-6.5172172137177272E-3</v>
       </c>
     </row>
     <row r="199" spans="1:1">
@@ -1357,27 +1357,27 @@
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
-        <v>1.2767793433949327E-3</v>
+        <v>1.2767793433949325E-3</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
-        <v>-1.3873300320145422E-2</v>
+        <v>-1.3873300320145424E-2</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
-        <v>1.5211649234838846E-3</v>
+        <v>1.5211649234838844E-3</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
-        <v>-1.8492737110793259E-3</v>
+        <v>-1.8492737110793256E-3</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
-        <v>-2.5525164724148321E-2</v>
+        <v>-2.5525164724148317E-2</v>
       </c>
     </row>
     <row r="206" spans="1:1">
@@ -1387,7 +1387,7 @@
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
-        <v>2.6905127829469789E-2</v>
+        <v>2.6905127829469785E-2</v>
       </c>
     </row>
     <row r="208" spans="1:1">
@@ -1397,7 +1397,7 @@
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
-        <v>-2.9017471080112602E-3</v>
+        <v>-2.9017471080112598E-3</v>
       </c>
     </row>
     <row r="210" spans="1:1">
@@ -1407,7 +1407,7 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
-        <v>-2.3018042570493967E-2</v>
+        <v>-2.301804257049397E-2</v>
       </c>
     </row>
     <row r="212" spans="1:1">
@@ -1417,7 +1417,7 @@
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
-        <v>1.1541873307683016E-2</v>
+        <v>1.1541873307683017E-2</v>
       </c>
     </row>
     <row r="214" spans="1:1">
@@ -1432,7 +1432,7 @@
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
-        <v>3.568728572174508E-3</v>
+        <v>3.5687285721745085E-3</v>
       </c>
     </row>
     <row r="217" spans="1:1">
@@ -1457,17 +1457,17 @@
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
-        <v>8.0683998426131793E-3</v>
+        <v>8.068399842613181E-3</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <v>1.0512258225195475E-2</v>
+        <v>1.0512258225195473E-2</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <v>8.7166896874507269E-4</v>
+        <v>8.716689687450728E-4</v>
       </c>
     </row>
     <row r="224" spans="1:1">
@@ -1492,7 +1492,7 @@
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
-        <v>1.7938176898980866E-3</v>
+        <v>1.7938176898980871E-3</v>
       </c>
     </row>
     <row r="229" spans="1:1">
@@ -1532,7 +1532,7 @@
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
-        <v>3.5491929776832773E-3</v>
+        <v>3.5491929776832768E-3</v>
       </c>
     </row>
     <row r="237" spans="1:1">
@@ -1552,17 +1552,17 @@
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
-        <v>1.783296929119213E-3</v>
+        <v>1.7832969291192132E-3</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
-        <v>1.0332964171403502E-3</v>
+        <v>1.0332964171403504E-3</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242">
-        <v>-7.0195327536904436E-3</v>
+        <v>-7.0195327536904445E-3</v>
       </c>
     </row>
     <row r="243" spans="1:1">
@@ -1572,7 +1572,7 @@
     </row>
     <row r="244" spans="1:1">
       <c r="A244">
-        <v>-9.2602466462088102E-4</v>
+        <v>-9.2602466462088091E-4</v>
       </c>
     </row>
     <row r="245" spans="1:1">
@@ -1587,7 +1587,7 @@
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
-        <v>-3.0122381115260158E-3</v>
+        <v>-3.0122381115260163E-3</v>
       </c>
     </row>
     <row r="248" spans="1:1">
@@ -1612,7 +1612,7 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
-        <v>1.2634173478362362E-2</v>
+        <v>1.2634173478362364E-2</v>
       </c>
     </row>
     <row r="253" spans="1:1">
@@ -1627,17 +1627,17 @@
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
-        <v>4.5610862190897002E-3</v>
+        <v>4.5610862190896993E-3</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
-        <v>8.0787794520398933E-4</v>
+        <v>8.0787794520398922E-4</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257">
-        <v>8.3822240974065626E-3</v>
+        <v>8.3822240974065643E-3</v>
       </c>
     </row>
     <row r="258" spans="1:1">
@@ -1657,7 +1657,7 @@
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
-        <v>1.6268487440785238E-3</v>
+        <v>1.6268487440785236E-3</v>
       </c>
     </row>
     <row r="262" spans="1:1">
@@ -1667,7 +1667,7 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
-        <v>2.522232774353031E-3</v>
+        <v>2.5222327743530306E-3</v>
       </c>
     </row>
     <row r="264" spans="1:1">
@@ -1682,32 +1682,32 @@
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
-        <v>-4.060332499652596E-3</v>
+        <v>-4.0603324996525952E-3</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
-        <v>1.7648744034247999E-3</v>
+        <v>1.7648744034247997E-3</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268">
-        <v>-6.4525473912899608E-3</v>
+        <v>-6.4525473912899617E-3</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269">
-        <v>1.8094620153962053E-3</v>
+        <v>1.8094620153962055E-3</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270">
-        <v>-1.3754500207341274E-2</v>
+        <v>-1.3754500207341272E-2</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271">
-        <v>2.1727829901986967E-3</v>
+        <v>2.1727829901986963E-3</v>
       </c>
     </row>
     <row r="272" spans="1:1">
@@ -1752,7 +1752,7 @@
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
-        <v>3.3954185551004147E-3</v>
+        <v>3.3954185551004143E-3</v>
       </c>
     </row>
     <row r="281" spans="1:1">
@@ -1787,7 +1787,7 @@
     </row>
     <row r="287" spans="1:1">
       <c r="A287">
-        <v>-3.9571456315484902E-3</v>
+        <v>-3.957145631548491E-3</v>
       </c>
     </row>
     <row r="288" spans="1:1">
@@ -1817,7 +1817,7 @@
     </row>
     <row r="293" spans="1:1">
       <c r="A293">
-        <v>-5.7669445508632504E-3</v>
+        <v>-5.7669445508632495E-3</v>
       </c>
     </row>
     <row r="294" spans="1:1">
@@ -1827,7 +1827,7 @@
     </row>
     <row r="295" spans="1:1">
       <c r="A295">
-        <v>-9.0943976256653819E-4</v>
+        <v>-9.0943976256653829E-4</v>
       </c>
     </row>
     <row r="296" spans="1:1">
@@ -1837,7 +1837,7 @@
     </row>
     <row r="297" spans="1:1">
       <c r="A297">
-        <v>4.5486944934666025E-3</v>
+        <v>4.5486944934666016E-3</v>
       </c>
     </row>
     <row r="298" spans="1:1">
@@ -1847,22 +1847,22 @@
     </row>
     <row r="299" spans="1:1">
       <c r="A299">
-        <v>2.8796959437176425E-3</v>
+        <v>2.8796959437176421E-3</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300">
-        <v>-2.8339762450559417E-4</v>
+        <v>-2.8339762450559422E-4</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301">
-        <v>-1.4672540648701326E-3</v>
+        <v>-1.4672540648701328E-3</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302">
-        <v>-7.1745906305176171E-3</v>
+        <v>-7.1745906305176162E-3</v>
       </c>
     </row>
     <row r="303" spans="1:1">
@@ -1887,7 +1887,7 @@
     </row>
     <row r="307" spans="1:1">
       <c r="A307">
-        <v>3.2859564718552238E-3</v>
+        <v>3.2859564718552233E-3</v>
       </c>
     </row>
     <row r="308" spans="1:1">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="309" spans="1:1">
       <c r="A309">
-        <v>2.0105569719813116E-3</v>
+        <v>2.010556971981312E-3</v>
       </c>
     </row>
     <row r="310" spans="1:1">
@@ -1927,7 +1927,7 @@
     </row>
     <row r="315" spans="1:1">
       <c r="A315">
-        <v>5.6436859813065359E-3</v>
+        <v>5.643685981306535E-3</v>
       </c>
     </row>
     <row r="316" spans="1:1">
@@ -1937,7 +1937,7 @@
     </row>
     <row r="317" spans="1:1">
       <c r="A317">
-        <v>-4.1364048443118717E-5</v>
+        <v>-4.1364048443118724E-5</v>
       </c>
     </row>
     <row r="318" spans="1:1">
@@ -1947,7 +1947,7 @@
     </row>
     <row r="319" spans="1:1">
       <c r="A319">
-        <v>-2.77593105340437E-3</v>
+        <v>-2.7759310534043705E-3</v>
       </c>
     </row>
     <row r="320" spans="1:1">
@@ -1967,12 +1967,12 @@
     </row>
     <row r="323" spans="1:1">
       <c r="A323">
-        <v>3.6875769198037151E-3</v>
+        <v>3.6875769198037147E-3</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324">
-        <v>3.0120430015099061E-4</v>
+        <v>3.0120430015099055E-4</v>
       </c>
     </row>
     <row r="325" spans="1:1">
@@ -2007,12 +2007,12 @@
     </row>
     <row r="331" spans="1:1">
       <c r="A331">
-        <v>-6.279756524520271E-4</v>
+        <v>-6.2797565245202699E-4</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332">
-        <v>-3.330760262288329E-3</v>
+        <v>-3.3307602622883294E-3</v>
       </c>
     </row>
     <row r="333" spans="1:1">
@@ -2027,12 +2027,12 @@
     </row>
     <row r="335" spans="1:1">
       <c r="A335">
-        <v>2.6560440581162104E-3</v>
+        <v>2.65604405811621E-3</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336">
-        <v>-6.863158908838689E-5</v>
+        <v>-6.8631589088386904E-5</v>
       </c>
     </row>
     <row r="337" spans="1:1">
@@ -2042,17 +2042,17 @@
     </row>
     <row r="338" spans="1:1">
       <c r="A338">
-        <v>-4.7192233991809611E-4</v>
+        <v>-4.7192233991809617E-4</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339">
-        <v>7.2147238197866205E-4</v>
+        <v>7.2147238197866194E-4</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340">
-        <v>-8.2303013971090442E-3</v>
+        <v>-8.2303013971090459E-3</v>
       </c>
     </row>
     <row r="341" spans="1:1">
@@ -2067,7 +2067,7 @@
     </row>
     <row r="343" spans="1:1">
       <c r="A343">
-        <v>-1.5090310549776571E-3</v>
+        <v>-1.5090310549776568E-3</v>
       </c>
     </row>
     <row r="344" spans="1:1">
@@ -2077,7 +2077,7 @@
     </row>
     <row r="345" spans="1:1">
       <c r="A345">
-        <v>-2.107494212706525E-2</v>
+        <v>-2.1074942127065246E-2</v>
       </c>
     </row>
     <row r="346" spans="1:1">
@@ -2102,7 +2102,7 @@
     </row>
     <row r="350" spans="1:1">
       <c r="A350">
-        <v>-1.4304959469482112E-2</v>
+        <v>-1.430495946948211E-2</v>
       </c>
     </row>
     <row r="351" spans="1:1">
@@ -2122,7 +2122,7 @@
     </row>
     <row r="354" spans="1:1">
       <c r="A354">
-        <v>-3.1246462129227163E-2</v>
+        <v>-3.1246462129227159E-2</v>
       </c>
     </row>
     <row r="355" spans="1:1">
@@ -2132,12 +2132,12 @@
     </row>
     <row r="356" spans="1:1">
       <c r="A356">
-        <v>-1.7711258725974441E-2</v>
+        <v>-1.7711258725974444E-2</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357">
-        <v>-6.4347007799340937E-3</v>
+        <v>-6.4347007799340928E-3</v>
       </c>
     </row>
     <row r="358" spans="1:1">
@@ -2172,7 +2172,7 @@
     </row>
     <row r="364" spans="1:1">
       <c r="A364">
-        <v>2.0916621479114619E-2</v>
+        <v>2.0916621479114623E-2</v>
       </c>
     </row>
     <row r="365" spans="1:1">
@@ -2182,17 +2182,17 @@
     </row>
     <row r="366" spans="1:1">
       <c r="A366">
-        <v>-9.3241686542832811E-3</v>
+        <v>-9.3241686542832828E-3</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367">
-        <v>-1.9727184498523648E-2</v>
+        <v>-1.9727184498523651E-2</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368">
-        <v>-1.6040791824065924E-3</v>
+        <v>-1.6040791824065927E-3</v>
       </c>
     </row>
     <row r="369" spans="1:1">
@@ -2202,7 +2202,7 @@
     </row>
     <row r="370" spans="1:1">
       <c r="A370">
-        <v>1.0507539140570869E-2</v>
+        <v>1.0507539140570871E-2</v>
       </c>
     </row>
     <row r="371" spans="1:1">
@@ -2212,12 +2212,12 @@
     </row>
     <row r="372" spans="1:1">
       <c r="A372">
-        <v>-1.6848368831321701E-2</v>
+        <v>-1.6848368831321698E-2</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373">
-        <v>-1.8427116011653956E-2</v>
+        <v>-1.8427116011653959E-2</v>
       </c>
     </row>
     <row r="374" spans="1:1">
@@ -2227,22 +2227,22 @@
     </row>
     <row r="375" spans="1:1">
       <c r="A375">
-        <v>-6.5764677658551214E-3</v>
+        <v>-6.5764677658551223E-3</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376">
-        <v>1.5469122069940913E-2</v>
+        <v>1.5469122069940911E-2</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377">
-        <v>3.2301156757264683E-3</v>
+        <v>3.2301156757264678E-3</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378">
-        <v>2.2724271516164615E-2</v>
+        <v>2.2724271516164619E-2</v>
       </c>
     </row>
     <row r="379" spans="1:1">
@@ -2257,7 +2257,7 @@
     </row>
     <row r="381" spans="1:1">
       <c r="A381">
-        <v>1.1335068139005464E-2</v>
+        <v>1.1335068139005465E-2</v>
       </c>
     </row>
     <row r="382" spans="1:1">
@@ -2267,7 +2267,7 @@
     </row>
     <row r="383" spans="1:1">
       <c r="A383">
-        <v>-1.8122022840641686E-3</v>
+        <v>-1.8122022840641684E-3</v>
       </c>
     </row>
     <row r="384" spans="1:1">
@@ -2277,32 +2277,32 @@
     </row>
     <row r="385" spans="1:1">
       <c r="A385">
-        <v>1.7076506881930581E-3</v>
+        <v>1.7076506881930583E-3</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386">
-        <v>-1.9338729278239238E-4</v>
+        <v>-1.9338729278239235E-4</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387">
-        <v>5.4761915551570376E-3</v>
+        <v>5.4761915551570367E-3</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388">
-        <v>-4.7533000491318568E-4</v>
+        <v>-4.7533000491318573E-4</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389">
-        <v>-1.902780453743514E-2</v>
+        <v>-1.9027804537435144E-2</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390">
-        <v>-2.1041217130882851E-2</v>
+        <v>-2.1041217130882847E-2</v>
       </c>
     </row>
     <row r="391" spans="1:1">
@@ -2312,12 +2312,12 @@
     </row>
     <row r="392" spans="1:1">
       <c r="A392">
-        <v>-1.5504247905780644E-2</v>
+        <v>-1.5504247905780645E-2</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393">
-        <v>-1.6105091252918178E-2</v>
+        <v>-1.6105091252918181E-2</v>
       </c>
     </row>
     <row r="394" spans="1:1">
@@ -2327,12 +2327,12 @@
     </row>
     <row r="395" spans="1:1">
       <c r="A395">
-        <v>-2.7341725050543286E-2</v>
+        <v>-2.7341725050543282E-2</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396">
-        <v>4.8395134248375639E-2</v>
+        <v>4.8395134248375632E-2</v>
       </c>
     </row>
     <row r="397" spans="1:1">
@@ -2357,12 +2357,12 @@
     </row>
     <row r="401" spans="1:1">
       <c r="A401">
-        <v>-2.4995956322236501E-2</v>
+        <v>-2.4995956322236505E-2</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402">
-        <v>3.365192392002795E-2</v>
+        <v>3.3651923920027957E-2</v>
       </c>
     </row>
     <row r="403" spans="1:1">
@@ -2397,17 +2397,17 @@
     </row>
     <row r="409" spans="1:1">
       <c r="A409">
-        <v>1.082374202523558E-2</v>
+        <v>1.0823742025235582E-2</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410">
-        <v>2.0972391497030636E-3</v>
+        <v>2.0972391497030641E-3</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411">
-        <v>7.7119002070858847E-3</v>
+        <v>7.7119002070858839E-3</v>
       </c>
     </row>
     <row r="412" spans="1:1">
@@ -2452,17 +2452,17 @@
     </row>
     <row r="420" spans="1:1">
       <c r="A420">
-        <v>8.5300003068591711E-3</v>
+        <v>8.5300003068591729E-3</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421">
-        <v>6.4689630660214373E-4</v>
+        <v>6.4689630660214362E-4</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422">
-        <v>6.8975568672775441E-3</v>
+        <v>6.8975568672775449E-3</v>
       </c>
     </row>
     <row r="423" spans="1:1">
@@ -2477,7 +2477,7 @@
     </row>
     <row r="425" spans="1:1">
       <c r="A425">
-        <v>-9.4523181360854618E-3</v>
+        <v>-9.4523181360854601E-3</v>
       </c>
     </row>
     <row r="426" spans="1:1">
@@ -2512,7 +2512,7 @@
     </row>
     <row r="432" spans="1:1">
       <c r="A432">
-        <v>1.5479990707235663E-3</v>
+        <v>1.5479990707235665E-3</v>
       </c>
     </row>
     <row r="433" spans="1:1">
@@ -2522,7 +2522,7 @@
     </row>
     <row r="434" spans="1:1">
       <c r="A434">
-        <v>-3.6329145684647801E-3</v>
+        <v>-3.6329145684647797E-3</v>
       </c>
     </row>
     <row r="435" spans="1:1">
@@ -2537,7 +2537,7 @@
     </row>
     <row r="437" spans="1:1">
       <c r="A437">
-        <v>-8.8372256864454701E-4</v>
+        <v>-8.837225686445469E-4</v>
       </c>
     </row>
     <row r="438" spans="1:1">
@@ -2557,12 +2557,12 @@
     </row>
     <row r="441" spans="1:1">
       <c r="A441">
-        <v>-3.8556899469238889E-3</v>
+        <v>-3.8556899469238894E-3</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442">
-        <v>-1.2144553908594174E-3</v>
+        <v>-1.2144553908594172E-3</v>
       </c>
     </row>
     <row r="443" spans="1:1">
@@ -2577,12 +2577,12 @@
     </row>
     <row r="445" spans="1:1">
       <c r="A445">
-        <v>-2.148643176007096E-3</v>
+        <v>-2.1486431760070956E-3</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446">
-        <v>1.4567255837467747E-2</v>
+        <v>1.4567255837467746E-2</v>
       </c>
     </row>
     <row r="447" spans="1:1">
@@ -2602,12 +2602,12 @@
     </row>
     <row r="450" spans="1:1">
       <c r="A450">
-        <v>4.9191285979491781E-3</v>
+        <v>4.9191285979491789E-3</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451">
-        <v>3.7485412223093929E-3</v>
+        <v>3.7485412223093924E-3</v>
       </c>
     </row>
     <row r="452" spans="1:1">
@@ -2622,12 +2622,12 @@
     </row>
     <row r="454" spans="1:1">
       <c r="A454">
-        <v>1.0892544443427321E-2</v>
+        <v>1.089254444342732E-2</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455">
-        <v>-1.9166413548224907E-2</v>
+        <v>-1.916641354822491E-2</v>
       </c>
     </row>
     <row r="456" spans="1:1">
@@ -2652,7 +2652,7 @@
     </row>
     <row r="460" spans="1:1">
       <c r="A460">
-        <v>6.694173901362759E-3</v>
+        <v>6.6941739013627582E-3</v>
       </c>
     </row>
     <row r="461" spans="1:1">
@@ -2672,17 +2672,17 @@
     </row>
     <row r="464" spans="1:1">
       <c r="A464">
-        <v>2.1450842530637954E-3</v>
+        <v>2.1450842530637958E-3</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465">
-        <v>4.57376500287644E-3</v>
+        <v>4.5737650028764409E-3</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466">
-        <v>1.0503948584247253E-3</v>
+        <v>1.0503948584247255E-3</v>
       </c>
     </row>
     <row r="467" spans="1:1">
@@ -2692,7 +2692,7 @@
     </row>
     <row r="468" spans="1:1">
       <c r="A468">
-        <v>3.4228141039660529E-3</v>
+        <v>3.4228141039660534E-3</v>
       </c>
     </row>
     <row r="469" spans="1:1">
@@ -2702,17 +2702,17 @@
     </row>
     <row r="470" spans="1:1">
       <c r="A470">
-        <v>6.6012306843098861E-3</v>
+        <v>6.6012306843098853E-3</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471">
-        <v>-6.8122471695493717E-4</v>
+        <v>-6.8122471695493728E-4</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472">
-        <v>5.5396040083746515E-4</v>
+        <v>5.5396040083746526E-4</v>
       </c>
     </row>
     <row r="473" spans="1:1">
@@ -2722,7 +2722,7 @@
     </row>
     <row r="474" spans="1:1">
       <c r="A474">
-        <v>1.6260390249190142E-3</v>
+        <v>1.6260390249190145E-3</v>
       </c>
     </row>
     <row r="475" spans="1:1">
@@ -2752,22 +2752,22 @@
     </row>
     <row r="480" spans="1:1">
       <c r="A480">
-        <v>1.1117326323400233E-3</v>
+        <v>1.111732632340023E-3</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481">
-        <v>7.6084117375281959E-4</v>
+        <v>7.608411737528197E-4</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482">
-        <v>-7.3848607577170775E-3</v>
+        <v>-7.3848607577170784E-3</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483">
-        <v>-2.0544012484873019E-3</v>
+        <v>-2.0544012484873023E-3</v>
       </c>
     </row>
     <row r="484" spans="1:1">
@@ -2792,12 +2792,12 @@
     </row>
     <row r="488" spans="1:1">
       <c r="A488">
-        <v>-3.1754946870729875E-3</v>
+        <v>-3.175494687072988E-3</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489">
-        <v>3.8975289109259986E-3</v>
+        <v>3.8975289109259982E-3</v>
       </c>
     </row>
     <row r="490" spans="1:1">
@@ -2807,12 +2807,12 @@
     </row>
     <row r="491" spans="1:1">
       <c r="A491">
-        <v>8.0936251045052397E-3</v>
+        <v>8.0936251045052379E-3</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492">
-        <v>5.8285000919236088E-3</v>
+        <v>5.828500091923608E-3</v>
       </c>
     </row>
     <row r="493" spans="1:1">
@@ -2822,7 +2822,7 @@
     </row>
     <row r="494" spans="1:1">
       <c r="A494">
-        <v>-5.9800970095067359E-3</v>
+        <v>-5.9800970095067367E-3</v>
       </c>
     </row>
     <row r="495" spans="1:1">
@@ -2842,12 +2842,12 @@
     </row>
     <row r="498" spans="1:1">
       <c r="A498">
-        <v>-1.1953877093569987E-2</v>
+        <v>-1.1953877093569985E-2</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499">
-        <v>1.5436418134818905E-3</v>
+        <v>1.5436418134818907E-3</v>
       </c>
     </row>
     <row r="500" spans="1:1">
@@ -2857,7 +2857,7 @@
     </row>
     <row r="501" spans="1:1">
       <c r="A501">
-        <v>-6.8869093749149906E-3</v>
+        <v>-6.8869093749149898E-3</v>
       </c>
     </row>
     <row r="502" spans="1:1">

</xml_diff>